<commit_message>
more details for study endpoints
</commit_message>
<xml_diff>
--- a/POLE_tmp/Meta-Analysis/data_extraction.xlsx
+++ b/POLE_tmp/Meta-Analysis/data_extraction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="18980" yWindow="4140" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,22 +104,211 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
-    <t xml:space="preserve">recurrenct, death, cancer-specific                                   </t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>death, recurrence</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>relapse, overall</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">distant metastasis, recurrence-free, and overall survival </t>
-  </si>
-  <si>
-    <t>overall, progression-free</t>
+    <t>Progressive-free survival: time to clinical/radiological evidence of disease progression from initial diagnosis, Disease-specific survival (DSS): time to death from disease excluding death from other causes, and Overall survival</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as PORTEC1, but measured from time of biopsy diagnosis to the death of patients </t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as PORTEC1, but measured from time of diagnosis</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>progression-free survival</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progression-free survival (PFS): time from surgery to first recurrence or death from disease; Overall survival (OS): time from surgery to death from any cause</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distant metastasis free survival; Recurrence-free survival: date of diagnosis to local, regional, or distant recurrences; Overall survival: date of diagnosis to all deaths irrespective of cause</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recurrence-free survival (RFS): time from random assignment to relapse, with censoring at last contact or death in case of no recurrence; Cancer-specific survival (CSS): time from random assign- ment to death from EC, with censoring at date of last contact or noncancer death; Overall survival (OS): ime from random assignment to death from any cause, with censoring at date of last contact in patients still alive</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same as PORTEC1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>32 months</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>low-grade endometrioid, high-grade endometrioid, and serous carcinomas</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>primary</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this study, the frequency, spectrum, prognostic significance, and potentialclinical application of POLE mutations were investigated in patients with endometrioid EC.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>USA</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>June 1990 - December 1997</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>May 2002 - September 2006</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>159.6 months</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>89 months</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>29 months</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrospective cohort</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>secondary</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>46 months</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>older patients or high stage and endometrioid</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>or grade 3 EECs and NEECs</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Church 2015</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Cohorts</t>
+  </si>
+  <si>
+    <t>Portec 1</t>
+  </si>
+  <si>
+    <t>Portec 2</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>considered N</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>Intermediate risk</t>
+  </si>
+  <si>
+    <t>Primary aim of study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postoperative pelvic radiotherapy improves locoregional control and survival for patients with stage-1 endometrial carcinoma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This study established whether vaginal brachytherapy (VBT) is as effective as pelvic external beam radiotherapy (EBRT) in prevention of vaginal recurrence, with fewer adverse effects and improved quality of life. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leuven </t>
+  </si>
+  <si>
+    <t>Tyoe of cohort</t>
+  </si>
+  <si>
+    <t>prospective RCT</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Age of cohort</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>August 95- September 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endometrial cancer patients may benefit from systemic adjuvant chemotherapy, alone or in com- bination with targeted therapies. Prognostic and predictive markers are needed, however, to identify patients amenable for these therapies. </t>
+  </si>
+  <si>
+    <t>Case control retrospective</t>
+  </si>
+  <si>
+    <t>endpoints</t>
+  </si>
+  <si>
+    <t>type of data</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>Protec (combined)</t>
+  </si>
+  <si>
+    <t>TCGA 2013</t>
+  </si>
+  <si>
+    <t>TGCA</t>
+  </si>
+  <si>
+    <t>Billingsley 2014</t>
+  </si>
+  <si>
+    <t>Portec 3</t>
+  </si>
+  <si>
+    <t>https://www.clinicalresearch.nl/portec3/</t>
+  </si>
+  <si>
+    <t>Bo Meng</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Calgary clear cells</t>
+  </si>
+  <si>
+    <t>Hoang</t>
+  </si>
+  <si>
+    <t>primary</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>68.4 months for EDM and 70.6 months for wildtype</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -127,14 +316,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>cancer-specific</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>progression-free, disease-specific, and ovreall survival</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>September 2006 - December 2015</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -238,185 +419,6 @@
   </si>
   <si>
     <t>Stello 2015</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>32 months</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>low-grade endometrioid, high-grade endometrioid, and serous carcinomas</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>primary</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>In this study, the frequency, spectrum, prognostic significance, and potentialclinical application of POLE mutations were investigated in patients with endometrioid EC.</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>USA</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>June 1990 - December 1997</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>May 2002 - September 2006</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>159.6 months</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>89 months</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>29 months</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>retrospective cohort</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>secondary</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>46 months</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>older patients or high stage and endometrioid</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>or grade 3 EECs and NEECs</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Church 2015</t>
-  </si>
-  <si>
-    <t>Paper</t>
-  </si>
-  <si>
-    <t>Cohorts</t>
-  </si>
-  <si>
-    <t>Portec 1</t>
-  </si>
-  <si>
-    <t>Portec 2</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>considered N</t>
-  </si>
-  <si>
-    <t>selection</t>
-  </si>
-  <si>
-    <t>Intermediate risk</t>
-  </si>
-  <si>
-    <t>Primary aim of study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postoperative pelvic radiotherapy improves locoregional control and survival for patients with stage-1 endometrial carcinoma </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This study established whether vaginal brachytherapy (VBT) is as effective as pelvic external beam radiotherapy (EBRT) in prevention of vaginal recurrence, with fewer adverse effects and improved quality of life. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leuven </t>
-  </si>
-  <si>
-    <t>Tyoe of cohort</t>
-  </si>
-  <si>
-    <t>prospective RCT</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Age of cohort</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>August 95- September 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endometrial cancer patients may benefit from systemic adjuvant chemotherapy, alone or in com- bination with targeted therapies. Prognostic and predictive markers are needed, however, to identify patients amenable for these therapies. </t>
-  </si>
-  <si>
-    <t>Case control retrospective</t>
-  </si>
-  <si>
-    <t>endpoints</t>
-  </si>
-  <si>
-    <t>death, death of disease, recurrence, relapse</t>
-  </si>
-  <si>
-    <t>type of data</t>
-  </si>
-  <si>
-    <t>primary</t>
-  </si>
-  <si>
-    <t>secondary</t>
-  </si>
-  <si>
-    <t>Protec (combined)</t>
-  </si>
-  <si>
-    <t>TCGA 2013</t>
-  </si>
-  <si>
-    <t>TGCA</t>
-  </si>
-  <si>
-    <t>Billingsley 2014</t>
-  </si>
-  <si>
-    <t>Portec 3</t>
-  </si>
-  <si>
-    <t>https://www.clinicalresearch.nl/portec3/</t>
-  </si>
-  <si>
-    <t>Bo Meng</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Calgary clear cells</t>
-  </si>
-  <si>
-    <t>Hoang</t>
-  </si>
-  <si>
-    <t>primary</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>68.4 months for EDM and 70.6 months for wildtype</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -849,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -865,63 +867,63 @@
     <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.6640625" customWidth="1"/>
+    <col min="11" max="11" width="153.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>434</v>
@@ -930,33 +932,33 @@
         <v>412</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>398</v>
@@ -965,38 +967,38 @@
         <v>376</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="F5">
         <v>187</v>
@@ -1005,33 +1007,33 @@
         <v>170</v>
       </c>
       <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
         <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" t="s">
-        <v>71</v>
       </c>
       <c r="K5" t="s">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="F6">
         <v>267</v>
@@ -1040,36 +1042,36 @@
         <v>229</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="F7">
         <v>373</v>
@@ -1078,36 +1080,36 @@
         <v>229</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>544</v>
@@ -1116,36 +1118,36 @@
         <v>535</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="K8" t="s">
         <v>4</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="F9">
         <v>116</v>
@@ -1154,36 +1156,36 @@
         <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>99</v>
@@ -1192,63 +1194,62 @@
         <v>99</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="K10" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="K11" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
added Stelloo paper, removed Hoang from meta-analysis
</commit_message>
<xml_diff>
--- a/POLE_tmp/Meta-Analysis/data_extraction.xlsx
+++ b/POLE_tmp/Meta-Analysis/data_extraction.xlsx
@@ -102,7 +102,205 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+  <si>
+    <t xml:space="preserve">tumour classification, which may have a direct effect on treatment recommendations for patients, and provides opportunities for genome-guided clinical trials and drug development </t>
+  </si>
+  <si>
+    <t>Various</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>November 1991 - January 2005</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>prospective cohort</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switzerland</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>The aim of this study is to further characterize the clinical and pathologic significance of POLE exonuclease domainmutations in high-grade endo- metrial carcinomas. Methods.We</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>primary</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Canada</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calgary (HGEC)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>2005 - 2011</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrospective cohort</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>high-grade endometrial carcinomas</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>36 months (45 months for censored cases)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>surgically staged endometrioid EC</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stello 2015</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>considered N</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>Intermediate risk</t>
+  </si>
+  <si>
+    <t>Primary aim of study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postoperative pelvic radiotherapy improves locoregional control and survival for patients with stage-1 endometrial carcinoma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This study established whether vaginal brachytherapy (VBT) is as effective as pelvic external beam radiotherapy (EBRT) in prevention of vaginal recurrence, with fewer adverse effects and improved quality of life. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leuven </t>
+  </si>
+  <si>
+    <t>Tyoe of cohort</t>
+  </si>
+  <si>
+    <t>prospective RCT</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Age of cohort</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>August 95- September 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endometrial cancer patients may benefit from systemic adjuvant chemotherapy, alone or in com- bination with targeted therapies. Prognostic and predictive markers are needed, however, to identify patients amenable for these therapies. </t>
+  </si>
+  <si>
+    <t>Case control retrospective</t>
+  </si>
+  <si>
+    <t>endpoints</t>
+  </si>
+  <si>
+    <t>type of data</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>Protec (combined)</t>
+  </si>
+  <si>
+    <t>TCGA 2013</t>
+  </si>
+  <si>
+    <t>TGCA</t>
+  </si>
+  <si>
+    <t>Billingsley 2014</t>
+  </si>
+  <si>
+    <t>Portec 3</t>
+  </si>
+  <si>
+    <t>https://www.clinicalresearch.nl/portec3/</t>
+  </si>
+  <si>
+    <t>Bo Meng</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>primary</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>68.4 months for EDM and 70.6 months for wildtype</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Median Follow-Up</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>September 2006 - December 2015</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>28.6 months</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>high risk endometrial carcinomas</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>prospective RCT</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigate whether molecular analysis can be used to refine risk assessment, direct adjuvant therapy, and identify actionable alterations in high-risk endometrial cancer </t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zurich and Basel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">To identify pathogenic factors and diagnostic markers for aggressive cases of endometrial carcinomas in general, irrespective of histological subtype </t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>type I and II endometrial carcinomas</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Some time around 2010</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
   <si>
     <t>Progressive-free survival: time to clinical/radiological evidence of disease progression from initial diagnosis, Disease-specific survival (DSS): time to death from disease excluding death from other causes, and Overall survival</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -209,217 +407,6 @@
   </si>
   <si>
     <t>Portec 2</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>considered N</t>
-  </si>
-  <si>
-    <t>selection</t>
-  </si>
-  <si>
-    <t>Intermediate risk</t>
-  </si>
-  <si>
-    <t>Primary aim of study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postoperative pelvic radiotherapy improves locoregional control and survival for patients with stage-1 endometrial carcinoma </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This study established whether vaginal brachytherapy (VBT) is as effective as pelvic external beam radiotherapy (EBRT) in prevention of vaginal recurrence, with fewer adverse effects and improved quality of life. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leuven </t>
-  </si>
-  <si>
-    <t>Tyoe of cohort</t>
-  </si>
-  <si>
-    <t>prospective RCT</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Age of cohort</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>August 95- September 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endometrial cancer patients may benefit from systemic adjuvant chemotherapy, alone or in com- bination with targeted therapies. Prognostic and predictive markers are needed, however, to identify patients amenable for these therapies. </t>
-  </si>
-  <si>
-    <t>Case control retrospective</t>
-  </si>
-  <si>
-    <t>endpoints</t>
-  </si>
-  <si>
-    <t>type of data</t>
-  </si>
-  <si>
-    <t>primary</t>
-  </si>
-  <si>
-    <t>secondary</t>
-  </si>
-  <si>
-    <t>Protec (combined)</t>
-  </si>
-  <si>
-    <t>TCGA 2013</t>
-  </si>
-  <si>
-    <t>TGCA</t>
-  </si>
-  <si>
-    <t>Billingsley 2014</t>
-  </si>
-  <si>
-    <t>Portec 3</t>
-  </si>
-  <si>
-    <t>https://www.clinicalresearch.nl/portec3/</t>
-  </si>
-  <si>
-    <t>Bo Meng</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Calgary clear cells</t>
-  </si>
-  <si>
-    <t>Hoang</t>
-  </si>
-  <si>
-    <t>primary</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>68.4 months for EDM and 70.6 months for wildtype</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Median Follow-Up</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>September 2006 - December 2015</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>28.6 months</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>high risk endometrial carcinomas</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>prospective RCT</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigate whether molecular analysis can be used to refine risk assessment, direct adjuvant therapy, and identify actionable alterations in high-risk endometrial cancer </t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zurich and Basel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">To identify pathogenic factors and diagnostic markers for aggressive cases of endometrial carcinomas in general, irrespective of histological subtype </t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>type I and II endometrial carcinomas</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Some time around 2010</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">tumour classification, which may have a direct effect on treatment recommendations for patients, and provides opportunities for genome-guided clinical trials and drug development </t>
-  </si>
-  <si>
-    <t>Various</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>?</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>November 1991 - January 2005</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>prospective cohort</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switzerland</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Endometrial clear cell carcinomas (CCC) con-stitute fewer than 5% of all carcinomas of the endo-metrium. Currently, little is known regarding thegenetic basis of endometrial CCC.</t>
-  </si>
-  <si>
-    <t>The aim of this study is to further characterize the clinical and pathologic significance of POLE exonuclease domainmutations in high-grade endo- metrial carcinomas. Methods.We</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>primary</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Canada</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Calgary (HGEC)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>2005 - 2011</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>retrospective cohort</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>high-grade endometrial carcinomas</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>36 months (45 months for censored cases)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>surgically staged endometrioid EC</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stello 2015</t>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -849,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -873,57 +860,57 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="F2">
         <v>434</v>
@@ -932,33 +919,33 @@
         <v>412</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="F3">
         <v>398</v>
@@ -967,38 +954,38 @@
         <v>376</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <v>187</v>
@@ -1007,33 +994,33 @@
         <v>170</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F6">
         <v>267</v>
@@ -1042,36 +1029,36 @@
         <v>229</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="K6" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <v>373</v>
@@ -1080,36 +1067,36 @@
         <v>229</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="L7" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="F8">
         <v>544</v>
@@ -1118,36 +1105,36 @@
         <v>535</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F9">
         <v>116</v>
@@ -1156,36 +1143,36 @@
         <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="K9" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>99</v>
@@ -1194,57 +1181,19 @@
         <v>99</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="L10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" t="s">
-        <v>74</v>
-      </c>
-      <c r="K11" t="s">
-        <v>74</v>
-      </c>
-      <c r="L11" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>